<commit_message>
started to add eyelink
</commit_message>
<xml_diff>
--- a/+ArumeExperimentDesigns/@IllusoryTilt/TrialTable.xlsx
+++ b/+ArumeExperimentDesigns/@IllusoryTilt/TrialTable.xlsx
@@ -534,8 +534,8 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CDA8567EE2FE4F4CBE3E2CEF37728AB4" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="944aec89eaeaf5cf1995eca05db96066">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="dab830d7-07ee-458a-b886-32578b44a612" xmlns:ns3="a048c95d-56bc-4d9d-b7f4-f756d5a4a43b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="36481b348f0f2de413f74f8a666e162d" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CDA8567EE2FE4F4CBE3E2CEF37728AB4" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f554a51c09cd52203fc280b1a67839d2">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="dab830d7-07ee-458a-b886-32578b44a612" xmlns:ns3="a048c95d-56bc-4d9d-b7f4-f756d5a4a43b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="58676131b01e20bbc69541e42ec7772b" ns2:_="" ns3:_="">
     <xsd:import namespace="dab830d7-07ee-458a-b886-32578b44a612"/>
     <xsd:import namespace="a048c95d-56bc-4d9d-b7f4-f756d5a4a43b"/>
     <xsd:element name="properties">
@@ -557,6 +557,9 @@
                 <xsd:element ref="ns3:MediaServiceKeyPoints" minOccurs="0"/>
                 <xsd:element ref="ns3:MediaServiceLocation" minOccurs="0"/>
                 <xsd:element ref="ns3:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns3:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns2:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceObjectDetectorVersions" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -593,6 +596,17 @@
         </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="23" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{35828c2f-142c-4d14-9ece-bbb868b00d38}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="dab830d7-07ee-458a-b886-32578b44a612">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="a048c95d-56bc-4d9d-b7f4-f756d5a4a43b" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -654,6 +668,18 @@
     <xsd:element name="MediaLengthInSeconds" ma:index="20" nillable="true" ma:displayName="Length (seconds)" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="22" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="fd1cee91-2f8e-42cc-b1e8-5796d73fb601" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="24" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:description="" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -758,7 +784,12 @@
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a048c95d-56bc-4d9d-b7f4-f756d5a4a43b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="dab830d7-07ee-458a-b886-32578b44a612" xsi:nil="true"/>
+  </documentManagement>
 </p:properties>
 </file>
 
@@ -771,7 +802,7 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EFA7EF9-819B-42E6-AF63-49C659E5AADB}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5196524-EC4E-4D8E-A0F2-A87C71DE12CE}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>